<commit_message>
Changes with cross browser and parallel testing
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Softwares\eclipse-workspace\automateTasks_POM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21068B69-FB97-4B11-B0A3-B67A57AC84B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD09A36-BDCA-499B-B186-F07DDD6ECAEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3E288751-3372-4148-9867-350E5C170502}"/>
   </bookViews>
@@ -46,18 +46,12 @@
     <t>Philips PowerPro FC9352</t>
   </si>
   <si>
-    <t>bejoise.antony.in@gmail.com</t>
-  </si>
-  <si>
     <t>Amazon#143</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Bejoise</t>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t>TC_Search_01</t>
+  </si>
+  <si>
+    <t>himabejo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Hima</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -475,13 +475,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -507,15 +507,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>